<commit_message>
update scrapper to be more flexible
</commit_message>
<xml_diff>
--- a/news_sites_and_title_class.xlsx
+++ b/news_sites_and_title_class.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NG8203C\Desktop\CodeBase\MyMedias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NG8203C\Desktop\CodeBase\News\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -161,6 +161,18 @@
   </si>
   <si>
     <t>class</t>
+  </si>
+  <si>
+    <t>date_published</t>
+  </si>
+  <si>
+    <t>title_text</t>
+  </si>
+  <si>
+    <t>title_text2</t>
+  </si>
+  <si>
+    <t>h3</t>
   </si>
 </sst>
 </file>
@@ -471,20 +483,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="26.54296875" customWidth="1"/>
     <col min="5" max="5" width="40.453125" customWidth="1"/>
-    <col min="7" max="7" width="22.7265625" customWidth="1"/>
+    <col min="6" max="7" width="14.90625" customWidth="1"/>
+    <col min="9" max="9" width="22.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,16 +514,25 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -526,8 +548,10 @@
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -541,8 +565,14 @@
       <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -556,8 +586,10 @@
       <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -573,8 +605,10 @@
       <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -590,11 +624,13 @@
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -605,14 +641,14 @@
       <c r="D7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -624,8 +660,10 @@
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
@@ -639,11 +677,13 @@
       <c r="E9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
@@ -657,6 +697,8 @@
       <c r="E10" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>